<commit_message>
insert testcase and update regresstion
</commit_message>
<xml_diff>
--- a/data/LoginF.xlsx
+++ b/data/LoginF.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -68,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +120,80 @@
       <b val="true"/>
       <color indexed="9"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +241,68 @@
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -247,11 +379,119 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -260,8 +500,20 @@
     <xf applyBorder="true" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="9" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="13" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="13" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="21" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="25" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="25" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="29" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="29" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="33" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" borderId="33" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="37" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -590,10 +842,10 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="21" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>